<commit_message>
added homework 3 solutions and grades to spreadsheet
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t xml:space="preserve">Homework 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 3</t>
   </si>
   <si>
     <t xml:space="preserve">Luka</t>
@@ -205,15 +211,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -234,121 +242,169 @@
       <c r="F2" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">12.5/17</f>
         <v>0.735294117647059</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">16/17</f>
         <v>0.941176470588235</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">14/17</f>
         <v>0.823529411764706</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">11/17</f>
         <v>0.647058823529412</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">14/17</f>
         <v>0.823529411764706</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">15/17</f>
         <v>0.882352941176471</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">14/17</f>
         <v>0.823529411764706</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>